<commit_message>
add several automation module crafting recipes
</commit_message>
<xml_diff>
--- a/project_resources/research/research_tree.xlsx
+++ b/project_resources/research/research_tree.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_source\git\AncientWarfare2\src\main\resources\data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="7860"/>
   </bookViews>
@@ -27,9 +22,10 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
     <author>John</author>
+    <author>Shadowmage</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0" shapeId="0">
+    <comment ref="C2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -53,7 +49,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0" shapeId="0">
+    <comment ref="E2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -77,7 +73,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0" shapeId="0">
+    <comment ref="G2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -101,7 +97,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0" shapeId="0">
+    <comment ref="C5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -127,7 +123,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0" shapeId="0">
+    <comment ref="E5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -153,7 +149,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0" shapeId="0">
+    <comment ref="G5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -178,7 +174,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0" shapeId="0">
+    <comment ref="C8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -202,7 +198,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0" shapeId="0">
+    <comment ref="E8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -226,7 +222,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0" shapeId="0">
+    <comment ref="G8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -250,7 +246,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0" shapeId="0">
+    <comment ref="C11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -274,7 +270,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="0" shapeId="0">
+    <comment ref="E11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -288,7 +284,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="0" shapeId="0">
+    <comment ref="I11" authorId="0">
       <text>
         <r>
           <rPr>
@@ -315,7 +311,21 @@
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0" shapeId="0">
+    <comment ref="A14" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">worker npcs
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -339,7 +349,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E14" authorId="0" shapeId="0">
+    <comment ref="E14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -351,7 +361,8 @@
           </rPr>
           <t>trader
 courier
-routing orders item</t>
+routing orders item
+warehouse</t>
         </r>
         <r>
           <rPr>
@@ -365,7 +376,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G14" authorId="0" shapeId="0">
+    <comment ref="G14" authorId="0">
       <text>
         <r>
           <rPr>
@@ -389,7 +400,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C17" authorId="0" shapeId="0">
+    <comment ref="C17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -413,7 +424,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E17" authorId="0" shapeId="0">
+    <comment ref="E17" authorId="0">
       <text>
         <r>
           <rPr>
@@ -2937,7 +2948,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2948,7 +2959,7 @@
   <dimension ref="A2:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add recipes for the rest of automation module. add icon for construction tool
</commit_message>
<xml_diff>
--- a/project_resources/research/research_tree.xlsx
+++ b/project_resources/research/research_tree.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -168,6 +168,30 @@
             <color indexed="81"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I5" authorId="1">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>heavy versions of torque blocks</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">
 </t>
@@ -2948,7 +2972,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2959,7 +2983,7 @@
   <dimension ref="A2:K17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
add icons for upgrade item(s).  update research tree spreadsheet to include most upgrades, rework tier of many worksites/etc NOTE: need to update recipe/research code to reflect sheet.
</commit_message>
<xml_diff>
--- a/project_resources/research/research_tree.xlsx
+++ b/project_resources/research/research_tree.xlsx
@@ -1,15 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_source\git\AncientWarfare2\project_resources\research\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="7860"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14940" windowHeight="7860" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +31,7 @@
     <author>Shadowmage</author>
   </authors>
   <commentList>
-    <comment ref="C2" authorId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -35,21 +41,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>hammer item</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <charset val="1"/>
-          </rPr>
-          <t xml:space="preserve">
-quill item</t>
+          <t xml:space="preserve">Quarry, hammer, quilll,
+</t>
         </r>
       </text>
     </comment>
-    <comment ref="E2" authorId="0">
+    <comment ref="C2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -59,7 +56,21 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>quarry</t>
+          <t>medium bounds</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>quarry medium bounds</t>
         </r>
         <r>
           <rPr>
@@ -73,7 +84,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G2" authorId="0">
+    <comment ref="G2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +108,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C5" authorId="0">
+    <comment ref="C5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -105,10 +116,9 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
-          <t>crop farm
-reed farm
+          <t>reed farm
 mushroom farm</t>
         </r>
         <r>
@@ -116,14 +126,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0">
+    <comment ref="E5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -149,7 +159,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G5" authorId="0">
+    <comment ref="G5" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -174,7 +184,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I5" authorId="1">
+    <comment ref="I5" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -182,7 +192,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>heavy versions of torque blocks</t>
         </r>
@@ -191,14 +201,29 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="C8" authorId="0">
+    <comment ref="A8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Farms
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -222,7 +247,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E8" authorId="0">
+    <comment ref="E8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -246,7 +271,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G8" authorId="0">
+    <comment ref="G8" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -270,7 +295,21 @@
         </r>
       </text>
     </comment>
-    <comment ref="C11" authorId="0">
+    <comment ref="I8" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>quarry large bounds</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -294,7 +333,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E11" authorId="0">
+    <comment ref="E11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -303,12 +342,12 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Work Orders Item
-</t>
+          <t>Work Orders Item
+large bounds</t>
         </r>
       </text>
     </comment>
-    <comment ref="I11" authorId="0">
+    <comment ref="I11" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -335,21 +374,21 @@
         </r>
       </text>
     </comment>
-    <comment ref="A14" authorId="1">
+    <comment ref="A14" authorId="1" shapeId="0">
       <text>
         <r>
           <rPr>
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">worker npcs
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="C14" authorId="0">
+    <comment ref="C14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -373,7 +412,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E14" authorId="0">
+    <comment ref="E14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -400,7 +439,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G14" authorId="0">
+    <comment ref="G14" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -424,7 +463,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C17" authorId="0">
+    <comment ref="C17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -448,7 +487,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E17" authorId="0">
+    <comment ref="E17" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -477,7 +516,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="104">
   <si>
     <t>Invention</t>
   </si>
@@ -564,13 +603,238 @@
   </si>
   <si>
     <t>Advanced Siege Warfare</t>
+  </si>
+  <si>
+    <t>Quarry</t>
+  </si>
+  <si>
+    <t>Hammer</t>
+  </si>
+  <si>
+    <t>Quill</t>
+  </si>
+  <si>
+    <t>Crop Farm</t>
+  </si>
+  <si>
+    <t>Workers</t>
+  </si>
+  <si>
+    <t>1st tier tech</t>
+  </si>
+  <si>
+    <t>2nd tier tech</t>
+  </si>
+  <si>
+    <t>Medium Work Bounds Upgrade</t>
+  </si>
+  <si>
+    <t>Requires Invention</t>
+  </si>
+  <si>
+    <t>Reed Farm</t>
+  </si>
+  <si>
+    <t>Mushroom Farm</t>
+  </si>
+  <si>
+    <t>Tree Farm</t>
+  </si>
+  <si>
+    <t>Requires Agriculture</t>
+  </si>
+  <si>
+    <t>Requires Leadership</t>
+  </si>
+  <si>
+    <t>TECH NAME</t>
+  </si>
+  <si>
+    <t>Pre-requisite tech</t>
+  </si>
+  <si>
+    <t>Unlocked Stuff</t>
+  </si>
+  <si>
+    <t>Animal Farm</t>
+  </si>
+  <si>
+    <t>Fish Farm</t>
+  </si>
+  <si>
+    <t>Combat Npcs</t>
+  </si>
+  <si>
+    <t>Command Baton</t>
+  </si>
+  <si>
+    <t>3rd tier tech</t>
+  </si>
+  <si>
+    <t>Requires Engineering</t>
+  </si>
+  <si>
+    <t>Requires Fishing</t>
+  </si>
+  <si>
+    <t>Requires Command</t>
+  </si>
+  <si>
+    <t>Quarry Medium Bounds Upgrade</t>
+  </si>
+  <si>
+    <t>Chest Cart (vehicle)</t>
+  </si>
+  <si>
+    <t>Hand-Cranked Engine</t>
+  </si>
+  <si>
+    <t>t1 Torque Conduits</t>
+  </si>
+  <si>
+    <t>Drafting Station</t>
+  </si>
+  <si>
+    <t>Large Work Bounds</t>
+  </si>
+  <si>
+    <t>Courier</t>
+  </si>
+  <si>
+    <t>Warehouse</t>
+  </si>
+  <si>
+    <t>Trader</t>
+  </si>
+  <si>
+    <t>Combat Orders Item</t>
+  </si>
+  <si>
+    <t>Routing Slip Item</t>
+  </si>
+  <si>
+    <t>Work Orders Item</t>
+  </si>
+  <si>
+    <t>Requires Conscription</t>
+  </si>
+  <si>
+    <t>4th tier tech</t>
+  </si>
+  <si>
+    <t>Requires Mining</t>
+  </si>
+  <si>
+    <t>Requires The Wheel</t>
+  </si>
+  <si>
+    <t>Sterling Generator</t>
+  </si>
+  <si>
+    <t>Clay Recipe</t>
+  </si>
+  <si>
+    <t>Gunpowder Recipe</t>
+  </si>
+  <si>
+    <t>Requires Construction</t>
+  </si>
+  <si>
+    <t>Requires Mathmatics</t>
+  </si>
+  <si>
+    <t>Flywheel Blocks</t>
+  </si>
+  <si>
+    <t>Waterwheel generator</t>
+  </si>
+  <si>
+    <t>Requires Trade</t>
+  </si>
+  <si>
+    <t>Basic Ships (vehicles)</t>
+  </si>
+  <si>
+    <t>5th tier tech</t>
+  </si>
+  <si>
+    <t>6th tier tech</t>
+  </si>
+  <si>
+    <t>Requires Combustion</t>
+  </si>
+  <si>
+    <t>Requires Chemistry</t>
+  </si>
+  <si>
+    <t>Steel</t>
+  </si>
+  <si>
+    <t>Heavy-duty torque blocks</t>
+  </si>
+  <si>
+    <t>Requires Theory of Gravity</t>
+  </si>
+  <si>
+    <t>Quarry Large Bounds Upgrade</t>
+  </si>
+  <si>
+    <t>Requires Seafaring</t>
+  </si>
+  <si>
+    <t>Mailbox</t>
+  </si>
+  <si>
+    <t>Advanced ships</t>
+  </si>
+  <si>
+    <t>Teleporter mechanics (undecided)</t>
+  </si>
+  <si>
+    <t>Requires Tactics</t>
+  </si>
+  <si>
+    <t>Basic Siege Engines (vehicles)</t>
+  </si>
+  <si>
+    <t>Requires Refining</t>
+  </si>
+  <si>
+    <t>Requires Explosives</t>
+  </si>
+  <si>
+    <t>Requires Machinery</t>
+  </si>
+  <si>
+    <t>Medium-duty torque blocks</t>
+  </si>
+  <si>
+    <t>Requires Navigation</t>
+  </si>
+  <si>
+    <t>Hot air baloon, gliders, ??</t>
+  </si>
+  <si>
+    <t>Advanced Siege Engines (vehicles)</t>
+  </si>
+  <si>
+    <t>Advanced warships (vehicles)</t>
+  </si>
+  <si>
+    <t>Basic Explosive Ammo</t>
+  </si>
+  <si>
+    <t>Advanced Explosive Ammo / rockets</t>
+  </si>
+  <si>
+    <t>Rockets?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -582,14 +846,7 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -599,18 +856,44 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -625,8 +908,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -837,15 +1126,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>733425</xdr:colOff>
+      <xdr:colOff>704850</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:rowOff>95250</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:colOff>571500</xdr:colOff>
       <xdr:row>7</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -854,8 +1143,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="733425" y="847725"/>
-          <a:ext cx="619125" cy="619125"/>
+          <a:off x="704850" y="857250"/>
+          <a:ext cx="1638300" cy="619125"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2972,7 +3261,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2982,13 +3271,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:K17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="26.5703125" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.140625" customWidth="1"/>
     <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
@@ -3102,4 +3391,490 @@
   <drawing r:id="rId2"/>
   <legacyDrawing r:id="rId3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F26" sqref="F26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="32.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" s="5"/>
+      <c r="I5" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="I8" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="I10" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A13" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G13" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="I13" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C14" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="I15" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="K15" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="A16" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K16" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E17" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I17" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C19" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="K19" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="20" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C20" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="K20" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="21" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E21" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="I22" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C23" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="24" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K24" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="G25" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K25" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="26" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C26" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="K26" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C27" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K27" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C28" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K28" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E29" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="I29" s="6" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C30" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="K30" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C31" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I31" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="K31" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C32" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="K33" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E34" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E35" s="6" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E36" s="6" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E37" s="6" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
+      <c r="E38" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add recipes and research for upgrades. Adjust research for some worksites to ease progression slightly (quarry and crop farm moved to lower tier)
</commit_message>
<xml_diff>
--- a/project_resources/research/research_tree.xlsx
+++ b/project_resources/research/research_tree.xlsx
@@ -13,7 +13,8 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="detail tree" sheetId="2" r:id="rId2"/>
+    <sheet name="research_by_item" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -516,7 +517,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="124">
   <si>
     <t>Invention</t>
   </si>
@@ -828,6 +829,66 @@
   </si>
   <si>
     <t>Rockets?</t>
+  </si>
+  <si>
+    <t>worker</t>
+  </si>
+  <si>
+    <t>combat npc</t>
+  </si>
+  <si>
+    <t>trader</t>
+  </si>
+  <si>
+    <t>courier</t>
+  </si>
+  <si>
+    <t>priest</t>
+  </si>
+  <si>
+    <t>combat order</t>
+  </si>
+  <si>
+    <t>work order</t>
+  </si>
+  <si>
+    <t>routing order</t>
+  </si>
+  <si>
+    <t>command baton</t>
+  </si>
+  <si>
+    <t>hammer</t>
+  </si>
+  <si>
+    <t>quill</t>
+  </si>
+  <si>
+    <t>Tool Quality 1 upgrade</t>
+  </si>
+  <si>
+    <t>Enchanted Tools 1 upgrade</t>
+  </si>
+  <si>
+    <t>Tool Quality 2 upgrade</t>
+  </si>
+  <si>
+    <t>Tool Quality 3 upgrade</t>
+  </si>
+  <si>
+    <t>Enchanted Tools 2 upgrade</t>
+  </si>
+  <si>
+    <t>Basic Chunkloader</t>
+  </si>
+  <si>
+    <t>Basic Chunkloader Upgrade</t>
+  </si>
+  <si>
+    <t>Quarry Chunkloader Upgrade</t>
+  </si>
+  <si>
+    <t>Deluxe Chunkloader</t>
   </si>
 </sst>
 </file>
@@ -3395,10 +3456,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O38"/>
+  <dimension ref="A1:O42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3477,7 +3538,7 @@
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>37</v>
@@ -3497,10 +3558,10 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="E9" s="4" t="s">
         <v>54</v>
@@ -3516,8 +3577,8 @@
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
-        <v>31</v>
+      <c r="C10" s="4" t="s">
+        <v>36</v>
       </c>
       <c r="G10" s="4" t="s">
         <v>70</v>
@@ -3530,8 +3591,11 @@
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C11" s="1" t="s">
-        <v>23</v>
+      <c r="A11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>115</v>
       </c>
       <c r="E11" s="1" t="s">
         <v>14</v>
@@ -3541,11 +3605,8 @@
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>41</v>
+      <c r="A12" s="4" t="s">
+        <v>32</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>51</v>
@@ -3558,11 +3619,8 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>37</v>
+      <c r="C13" s="1" t="s">
+        <v>23</v>
       </c>
       <c r="E13" s="4" t="s">
         <v>55</v>
@@ -3578,8 +3636,11 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="C14" s="4" t="s">
-        <v>38</v>
+      <c r="A14" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="E14" s="4" t="s">
         <v>56</v>
@@ -3595,11 +3656,11 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>39</v>
+      <c r="A15" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>37</v>
       </c>
       <c r="E15" s="4" t="s">
         <v>57</v>
@@ -3612,33 +3673,36 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>33</v>
-      </c>
       <c r="C16" s="4" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="I16" s="4" t="s">
+        <v>118</v>
+      </c>
       <c r="K16" s="4" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="17" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C17" s="4" t="s">
+        <v>39</v>
+      </c>
       <c r="E17" s="1" t="s">
         <v>3</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="I17" s="1" t="s">
-        <v>13</v>
+      <c r="K17" s="4" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C18" s="1" t="s">
-        <v>10</v>
+      <c r="C18" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>51</v>
@@ -3646,230 +3710,260 @@
       <c r="G18" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="I18" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>27</v>
+      <c r="I18" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C19" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="E19" s="4" t="s">
         <v>58</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="I19" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="K19" s="6" t="s">
-        <v>97</v>
+      <c r="I19" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="20" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C20" s="4" t="s">
-        <v>46</v>
+      <c r="C20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>117</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>75</v>
       </c>
+      <c r="I20" s="4" t="s">
+        <v>86</v>
+      </c>
       <c r="K20" s="6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="E21" s="1" t="s">
-        <v>11</v>
+      <c r="C21" s="6" t="s">
+        <v>41</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="I21" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="K21" s="4" t="s">
+      <c r="I21" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C22" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="K22" s="4" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C22" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E22" s="6" t="s">
+    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E23" s="6" t="s">
         <v>51</v>
-      </c>
-      <c r="I22" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="K22" s="4" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="23" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C23" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>65</v>
       </c>
       <c r="G23" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="I23" s="6" t="s">
-        <v>87</v>
+      <c r="K23" s="4" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="24" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C24" s="4" t="s">
-        <v>47</v>
+      <c r="C24" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="G24" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="I24" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="K24" s="1" t="s">
-        <v>9</v>
+      <c r="I24" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C25" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>59</v>
+      </c>
       <c r="G25" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="I25" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="K25" s="6" t="s">
-        <v>97</v>
+      <c r="I25" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="26" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>21</v>
+      <c r="C26" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>116</v>
       </c>
       <c r="G26" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="I26" s="4" t="s">
-        <v>90</v>
+      <c r="I26" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="K26" s="6" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C27" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>52</v>
+      <c r="E27" s="4" t="s">
+        <v>120</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>78</v>
       </c>
+      <c r="I27" s="4" t="s">
+        <v>88</v>
+      </c>
       <c r="K27" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="I28" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="K28" s="6" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="28" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C28" s="4" t="s">
+    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C29" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="I29" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="K29" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C30" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="E28" s="6" t="s">
+      <c r="E30" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E31" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K31" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C32" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="I28" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="K28" s="4" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="29" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="E29" s="4" t="s">
+      <c r="I32" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="K32" s="6" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C33" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E33" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="I29" s="6" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C30" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E30" s="4" t="s">
+      <c r="I33" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="K33" s="6" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="I30" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="K30" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C31" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E31" s="4" t="s">
+      <c r="I34" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="35" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E35" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="I31" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="K31" s="6" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="32" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C32" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="E32" s="4" t="s">
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E36" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="K32" s="6" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="33" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="K33" s="4" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="34" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E34" s="1" t="s">
+    </row>
+    <row r="38" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E38" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E35" s="6" t="s">
+    <row r="39" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E39" s="6" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="36" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E36" s="6" t="s">
+    <row r="40" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E40" s="6" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="37" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E37" s="6" t="s">
+    <row r="41" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E41" s="6" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="38" spans="5:11" x14ac:dyDescent="0.25">
-      <c r="E38" s="4" t="s">
+    <row r="42" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="E42" s="4" t="s">
         <v>63</v>
       </c>
     </row>
@@ -3877,4 +3971,74 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>114</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>